<commit_message>
update code and location of convert_to_cff.py
</commit_message>
<xml_diff>
--- a/templates/scores_and_POC_v20240315.xlsx
+++ b/templates/scores_and_POC_v20240315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsmit51\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/me/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E750FFE6-5565-4E01-98EE-96450C2662CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3280520F-0329-C84E-AA37-D48712F890B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{84F842C5-D660-4A9D-B934-A771036DE5AD}"/>
+    <workbookView xWindow="45340" yWindow="8160" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{84F842C5-D660-4A9D-B934-A771036DE5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Names and Logic" sheetId="2" r:id="rId1"/>
@@ -377,7 +377,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,12 +407,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -928,69 +922,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1012,79 +977,43 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1092,14 +1021,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,9 +1111,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1165,7 +1151,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1271,7 +1257,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1413,7 +1399,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1446,368 +1432,368 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="85.7109375" customWidth="1"/>
-    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.85546875" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="93.5703125" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.6640625" customWidth="1"/>
+    <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="85.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.83203125" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="93.5" customWidth="1"/>
+    <col min="13" max="13" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" t="s">
         <v>64</v>
       </c>
       <c r="O1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="28" t="str">
+      <c r="J2" s="27" t="str">
         <f>_xlfn.TEXTJOIN("::",FALSE,C2,E2,G2,I2)</f>
         <v>BMS::SD::REF::INHERIT</v>
       </c>
-      <c r="K2" s="28" t="str">
+      <c r="K2" s="27" t="str">
         <f>IF(COUNTIF(J:J,J2)&gt;1,"#NOT UNIQUE","Y")</f>
         <v>Y</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="28" t="str">
+      <c r="J3" s="27" t="str">
         <f>_xlfn.TEXTJOIN("::",FALSE,C3,E3,G3,I3)</f>
         <v>BMS::SD::EAMP::DESC</v>
       </c>
-      <c r="K3" s="28" t="str">
+      <c r="K3" s="27" t="str">
         <f t="shared" ref="K3:K9" si="0">IF(COUNTIF(J:J,J3)&gt;1,"#NOT UNIQUE","Y")</f>
         <v>Y</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="28" t="str">
+      <c r="J4" s="27" t="str">
         <f t="shared" ref="J4:J9" si="1">_xlfn.TEXTJOIN("::",FALSE,C4,E4,G4,I4)</f>
         <v>BMS::SD::EAMP::DOI</v>
       </c>
-      <c r="K4" s="28" t="str">
+      <c r="K4" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="28" t="str">
+      <c r="J5" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BMS::SND::EAMP::DESC</v>
       </c>
-      <c r="K5" s="28" t="str">
+      <c r="K5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="28" t="str">
+      <c r="J6" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BMS::SND::EAMP::DOI</v>
       </c>
-      <c r="K6" s="28" t="str">
+      <c r="K6" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="28" t="str">
+      <c r="J7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BMS::SND::NLP::DESC</v>
       </c>
-      <c r="K7" s="28" t="str">
+      <c r="K7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="28" t="str">
+      <c r="J8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BMS::SND::NLP::DOI</v>
       </c>
-      <c r="K8" s="28" t="str">
+      <c r="K8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="28" t="str">
+      <c r="J9" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BMS::INHERIT::INHERIT::INHERIT</v>
       </c>
-      <c r="K9" s="28" t="str">
+      <c r="K9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1815,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1823,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1831,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1839,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1847,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1855,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1871,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1879,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1887,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1895,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1903,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1911,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1919,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1935,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1943,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1951,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1959,17 +1945,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>4</v>
       </c>
@@ -1987,330 +1973,326 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="53" t="s">
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="71"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="62"/>
       <c r="N1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="str">
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="str">
         <f>_xlfn.XLOOKUP(H3,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B3" s="30" t="str">
+      <c r="B3" s="28" t="str">
         <f>_xlfn.XLOOKUP(H3,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>A: Study disseminated - reference</v>
       </c>
-      <c r="C3" s="73">
-        <v>1</v>
-      </c>
-      <c r="F3" s="74">
-        <v>1</v>
-      </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44" t="str">
+      <c r="C3" s="53">
+        <v>1</v>
+      </c>
+      <c r="F3" s="54">
+        <v>1</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33" t="str">
         <f>'Names and Logic'!J2</f>
         <v>BMS::SD::REF::INHERIT</v>
       </c>
-      <c r="I3" s="68" t="str">
+      <c r="I3" s="51" t="str">
         <f>IF(G3=1,H3,".")</f>
         <v>.</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="50">
         <f>IF(SUM(G3)&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="61">
+      <c r="K3" s="70">
         <f>IF(SUM(J3:J5)&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3" s="67">
         <f>IF(SUM(K3:K9)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="str">
         <f>_xlfn.XLOOKUP(H4,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B4" s="30" t="str">
+      <c r="B4" s="28" t="str">
         <f>_xlfn.XLOOKUP(H4,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>A: Study disseminated - evaluation and methods 1a - description</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="54">
         <v>2</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="54">
         <v>2</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45" t="str">
+      <c r="G4" s="34"/>
+      <c r="H4" s="34" t="str">
         <f>'Names and Logic'!J3</f>
         <v>BMS::SD::EAMP::DESC</v>
       </c>
-      <c r="I4" s="68" t="str">
+      <c r="I4" s="51" t="str">
         <f>IF(AND($G$3=1,G4=1),ERROR.TYPE(12),IF(G4=1,_xlfn.TEXTJOIN("::",FALSE,H4,G4),"."))</f>
         <v>.</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="80">
         <f>IF(SUM(G4:G5)&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="str">
+      <c r="K4" s="71"/>
+      <c r="L4" s="68"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="str">
         <f>_xlfn.XLOOKUP(H5,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B5" s="30" t="str">
+      <c r="B5" s="28" t="str">
         <f>_xlfn.XLOOKUP(H5,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>A: Study disseminated - evaluation and methods 1b - location</v>
       </c>
-      <c r="C5" s="74">
+      <c r="C5" s="54">
         <v>2</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="54">
         <v>2</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46" t="str">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35" t="str">
         <f>'Names and Logic'!J4</f>
         <v>BMS::SD::EAMP::DOI</v>
       </c>
-      <c r="I5" s="68" t="str">
+      <c r="I5" s="51" t="str">
         <f>IF(AND($G$3=1,G5=1),ERROR.TYPE(12),IF(G5=1,_xlfn.TEXTJOIN("::",FALSE,H5,G5),"."))</f>
         <v>.</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="str">
+      <c r="J5" s="81"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="str">
         <f>_xlfn.XLOOKUP(H6,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B6" s="30" t="str">
+      <c r="B6" s="28" t="str">
         <f>_xlfn.XLOOKUP(H6,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>B: Study not disseminated 1a - evaluation methods - description</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="54">
         <v>3</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="54">
         <v>3</v>
       </c>
-      <c r="G6" s="47">
-        <v>1</v>
-      </c>
-      <c r="H6" s="47" t="str">
+      <c r="G6" s="36"/>
+      <c r="H6" s="36" t="str">
         <f>'Names and Logic'!J5</f>
         <v>BMS::SND::EAMP::DESC</v>
       </c>
-      <c r="I6" s="68" t="str">
+      <c r="I6" s="51" t="str">
         <f>IF(AND(OR($G$3=1,$G$4=1,$G$5=1),G6=1),ERROR.TYPE(12),IF(G6=1,_xlfn.TEXTJOIN("::",FALSE,H6,G6),"."))</f>
-        <v>BMS::SND::EAMP::DESC::1</v>
-      </c>
-      <c r="J6" s="38">
+        <v>.</v>
+      </c>
+      <c r="J6" s="76">
         <f>IF(SUM(G6:G7)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="64">
+        <v>0</v>
+      </c>
+      <c r="K6" s="73">
         <f>IF(SUM(J6:J9)&gt;0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="str">
+        <v>0</v>
+      </c>
+      <c r="L6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="str">
         <f>_xlfn.XLOOKUP(H7,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B7" s="30" t="str">
+      <c r="B7" s="28" t="str">
         <f>_xlfn.XLOOKUP(H7,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>B: Study not disseminated 1b - evaluation methods - location</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="54">
         <v>3</v>
       </c>
-      <c r="F7" s="74">
+      <c r="F7" s="54">
         <v>3</v>
       </c>
-      <c r="G7" s="48">
-        <v>1</v>
-      </c>
-      <c r="H7" s="48" t="str">
+      <c r="G7" s="37"/>
+      <c r="H7" s="37" t="str">
         <f>'Names and Logic'!J6</f>
         <v>BMS::SND::EAMP::DOI</v>
       </c>
-      <c r="I7" s="60" t="str">
+      <c r="I7" s="49" t="str">
         <f>IF(AND(OR($G$3=1,$G$4=1,$G$5=1),G7=1),ERROR.TYPE(12),IF(G7=1,_xlfn.TEXTJOIN("::",FALSE,H7,G7),"."))</f>
-        <v>BMS::SND::EAMP::DOI::1</v>
-      </c>
-      <c r="J7" s="39"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="36"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="str">
+        <v>.</v>
+      </c>
+      <c r="J7" s="77"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="68"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="str">
         <f>_xlfn.XLOOKUP(H8,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B8" s="30" t="str">
+      <c r="B8" s="28" t="str">
         <f>_xlfn.XLOOKUP(H8,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>B: Study not disseminated 2a - nlp summary - description</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="54">
         <v>4</v>
       </c>
-      <c r="F8" s="74">
+      <c r="F8" s="54">
         <v>4</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49" t="str">
+      <c r="G8" s="38"/>
+      <c r="H8" s="38" t="str">
         <f>'Names and Logic'!J7</f>
         <v>BMS::SND::NLP::DESC</v>
       </c>
-      <c r="I8" s="60" t="str">
+      <c r="I8" s="49" t="str">
         <f>IF(AND(OR($G$3=1,$G$4=1,$G$5=1,$G$6=1,$G$7=1),G8=1),ERROR.TYPE(12),IF(G8=1,_xlfn.TEXTJOIN("::",FALSE,H8,G8),"."))</f>
         <v>.</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="78">
         <f>IF(SUM(G8:G9)&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="K8" s="65"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="str">
+      <c r="K8" s="74"/>
+      <c r="L8" s="68"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="str">
         <f>_xlfn.XLOOKUP(H9,'Names and Logic'!J:J,'Names and Logic'!B:B,"#NOT FOUND/MAPPED",0,1)</f>
         <v>Background Measurement Study or information availability</v>
       </c>
-      <c r="B9" s="31" t="str">
+      <c r="B9" s="29" t="str">
         <f>_xlfn.XLOOKUP(H9,'Names and Logic'!J:J,'Names and Logic'!A:A,"#NOT FOUND/MAPPED",0,1)</f>
         <v>B: Study not disseminated 2b - nlp summary - location</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="55">
         <v>4</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="55">
         <v>4</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50" t="str">
+      <c r="G9" s="39"/>
+      <c r="H9" s="39" t="str">
         <f>'Names and Logic'!J8</f>
         <v>BMS::SND::NLP::DOI</v>
       </c>
-      <c r="I9" s="60" t="str">
+      <c r="I9" s="49" t="str">
         <f>IF(AND(OR($G$3=1,$G$4=1,$G$5=1,$G$6=1,$G$7=1),G9=1),ERROR.TYPE(12),IF(G9=1,_xlfn.TEXTJOIN("::",FALSE,H9,G9),"."))</f>
         <v>.</v>
       </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="37"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I10" s="57" t="s">
+      <c r="J9" s="79"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="69"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I10" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="58" t="str">
+      <c r="J10" s="47" t="str">
         <f>IF(J3=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SD","REF",J3),IF(J4=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SD","EAMP",J4),IF(J6=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SND","EAMP",J6),IF(J8=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SND","NLP",J8),IF(AND(J3=0,J4=0,J6=0,J8=0),".","#ERROR IN FORMULA")))))</f>
-        <v>BMS::SND::EAMP::1</v>
-      </c>
-      <c r="K10" s="58" t="str">
+        <v>.</v>
+      </c>
+      <c r="K10" s="47" t="str">
         <f>IF(K3=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SD",K3),IF(K6=1,_xlfn.TEXTJOIN("::",FALSE,"BMS","SND",K6),IF(AND(K3=0,K6=0),".","#ERROR IN FORMULA")))</f>
-        <v>BMS::SND::1</v>
-      </c>
-      <c r="L10" s="58" t="str">
+        <v>.</v>
+      </c>
+      <c r="L10" s="47" t="str">
         <f>_xlfn.TEXTJOIN("::",FALSE,"BMS",L3)</f>
-        <v>BMS::1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="79" t="s">
+        <v>BMS::0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="77"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="83" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="56"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="78"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+      <c r="B13" s="66"/>
+      <c r="C13" s="57"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="82"/>
+      <c r="B14" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2344,14 +2326,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2368,7 +2350,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2386,7 +2368,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2386,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2401,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2452,7 +2434,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2485,188 +2467,188 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0</v>
       </c>
       <c r="D9">
         <v>25</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f>C10/D10*100</f>
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
         <v>20</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>5</v>
       </c>
       <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f>C12/D12*100</f>
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
         <v>3</v>
       </c>
       <c r="D14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
         <v>3</v>
       </c>
       <c r="D15">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17">
         <v>2</v>
       </c>
       <c r="D17">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2679,12 +2661,12 @@
       <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <f>C21/D21*100</f>
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2698,7 +2680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2712,7 +2694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2726,7 +2708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2740,7 +2722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2754,7 +2736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2768,7 +2750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2782,7 +2764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2796,17 +2778,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>

</xml_diff>